<commit_message>
Melhorando contornos e janela
Adicionado o botão Ajuda e Sobre;
TextBox apresenta mensagens e erros;
Logo do cursinho adicionado;
Botão Parar removido
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="179">
   <si>
     <t>w.jpeg</t>
   </si>
@@ -334,250 +334,211 @@
     <t>comErro3.jpeg</t>
   </si>
   <si>
+    <t>2.jpeg</t>
+  </si>
+  <si>
+    <t>Total: 50</t>
+  </si>
+  <si>
+    <t>1-A</t>
+  </si>
+  <si>
+    <t>21-E</t>
+  </si>
+  <si>
+    <t>Total: 0</t>
+  </si>
+  <si>
+    <t>testeComErro3.jpeg</t>
+  </si>
+  <si>
+    <t>gabarito.jpeg</t>
+  </si>
+  <si>
+    <t>iluminaçãoZoada2.jpeg</t>
+  </si>
+  <si>
+    <t>1-['D']</t>
+  </si>
+  <si>
+    <t>2-['C']</t>
+  </si>
+  <si>
+    <t>3-['E']</t>
+  </si>
+  <si>
+    <t>4-['A']</t>
+  </si>
+  <si>
+    <t>5-['A']</t>
+  </si>
+  <si>
+    <t>6-['C']</t>
+  </si>
+  <si>
+    <t>7-['E']</t>
+  </si>
+  <si>
+    <t>10-['B']</t>
+  </si>
+  <si>
+    <t>11-['E']</t>
+  </si>
+  <si>
+    <t>12-['C']</t>
+  </si>
+  <si>
+    <t>13-['A']</t>
+  </si>
+  <si>
+    <t>14-['E']</t>
+  </si>
+  <si>
+    <t>15-['C']</t>
+  </si>
+  <si>
+    <t>16-['B']</t>
+  </si>
+  <si>
+    <t>17-['E']</t>
+  </si>
+  <si>
+    <t>20-['A']</t>
+  </si>
+  <si>
+    <t>22-['E']</t>
+  </si>
+  <si>
+    <t>23-['B']</t>
+  </si>
+  <si>
+    <t>24-['D']</t>
+  </si>
+  <si>
+    <t>25-['B']</t>
+  </si>
+  <si>
+    <t>26-['E']</t>
+  </si>
+  <si>
+    <t>27-['A']</t>
+  </si>
+  <si>
+    <t>28-['C']</t>
+  </si>
+  <si>
+    <t>30-['E']</t>
+  </si>
+  <si>
+    <t>33-['A']</t>
+  </si>
+  <si>
+    <t>34-['E']</t>
+  </si>
+  <si>
+    <t>35-['B']</t>
+  </si>
+  <si>
+    <t>36-['C']</t>
+  </si>
+  <si>
+    <t>37-['D']</t>
+  </si>
+  <si>
+    <t>38-['A']</t>
+  </si>
+  <si>
+    <t>39-['D']</t>
+  </si>
+  <si>
+    <t>44-['A']</t>
+  </si>
+  <si>
+    <t>46-['B']</t>
+  </si>
+  <si>
+    <t>48-['-']</t>
+  </si>
+  <si>
+    <t>49-['B']</t>
+  </si>
+  <si>
+    <t>iluminaçãoZoada1.jpeg</t>
+  </si>
+  <si>
+    <t>Total: 2</t>
+  </si>
+  <si>
+    <t>Total: 4</t>
+  </si>
+  <si>
+    <t>2-['-']</t>
+  </si>
+  <si>
+    <t>3-['-']</t>
+  </si>
+  <si>
+    <t>4-['D']</t>
+  </si>
+  <si>
+    <t>meioZoado.png</t>
+  </si>
+  <si>
+    <t>gabaritoComErro.jpeg</t>
+  </si>
+  <si>
+    <t>1-['D', 'E']</t>
+  </si>
+  <si>
+    <t>20-['A', 'D', 'E']</t>
+  </si>
+  <si>
+    <t>3.jpeg</t>
+  </si>
+  <si>
+    <t>clahe_2.jpeg</t>
+  </si>
+  <si>
+    <t>Total: 7</t>
+  </si>
+  <si>
+    <t>Total: 43</t>
+  </si>
+  <si>
+    <t>23-['D', 'B']</t>
+  </si>
+  <si>
+    <t>41-['C']</t>
+  </si>
+  <si>
+    <t>45-['B']</t>
+  </si>
+  <si>
+    <t>47-['A']</t>
+  </si>
+  <si>
+    <t>48-['E']</t>
+  </si>
+  <si>
+    <t>testeComErro5.jpeg</t>
+  </si>
+  <si>
     <t>Total: 44</t>
   </si>
   <si>
     <t>Total: 6</t>
   </si>
   <si>
-    <t>23-['B', 'C']</t>
-  </si>
-  <si>
-    <t>2.jpeg</t>
-  </si>
-  <si>
-    <t>Total: 49</t>
-  </si>
-  <si>
-    <t>1-A</t>
-  </si>
-  <si>
-    <t>21-E</t>
-  </si>
-  <si>
-    <t>Total: 1</t>
-  </si>
-  <si>
-    <t>testeComErro3.jpeg</t>
-  </si>
-  <si>
-    <t>gabarito.jpeg</t>
-  </si>
-  <si>
-    <t>iluminaçãoZoada2.jpeg</t>
-  </si>
-  <si>
-    <t>1-['D']</t>
-  </si>
-  <si>
-    <t>2-['C']</t>
-  </si>
-  <si>
-    <t>3-['E', 'E']</t>
-  </si>
-  <si>
-    <t>4-['A']</t>
-  </si>
-  <si>
-    <t>5-['A', 'A']</t>
-  </si>
-  <si>
-    <t>6-['C']</t>
-  </si>
-  <si>
-    <t>7-['E', 'E']</t>
-  </si>
-  <si>
-    <t>10-['B']</t>
-  </si>
-  <si>
-    <t>11-['E']</t>
-  </si>
-  <si>
-    <t>12-['C']</t>
-  </si>
-  <si>
-    <t>13-['A']</t>
-  </si>
-  <si>
-    <t>14-['E']</t>
-  </si>
-  <si>
-    <t>15-['C']</t>
-  </si>
-  <si>
-    <t>16-['B']</t>
-  </si>
-  <si>
-    <t>17-['E']</t>
-  </si>
-  <si>
-    <t>20-['A']</t>
-  </si>
-  <si>
-    <t>22-['E']</t>
-  </si>
-  <si>
-    <t>23-['B']</t>
-  </si>
-  <si>
-    <t>24-['D']</t>
-  </si>
-  <si>
-    <t>25-['B', 'B']</t>
-  </si>
-  <si>
-    <t>26-['E', 'E']</t>
-  </si>
-  <si>
-    <t>27-['A']</t>
-  </si>
-  <si>
-    <t>28-['C']</t>
-  </si>
-  <si>
-    <t>30-['E']</t>
-  </si>
-  <si>
-    <t>33-['A']</t>
-  </si>
-  <si>
-    <t>34-['E']</t>
-  </si>
-  <si>
-    <t>35-['B']</t>
-  </si>
-  <si>
-    <t>36-['C']</t>
-  </si>
-  <si>
-    <t>37-['D']</t>
-  </si>
-  <si>
-    <t>38-['A']</t>
-  </si>
-  <si>
-    <t>39-['D']</t>
-  </si>
-  <si>
-    <t>44-['A']</t>
-  </si>
-  <si>
-    <t>46-['B']</t>
-  </si>
-  <si>
-    <t>48-['-']</t>
-  </si>
-  <si>
-    <t>49-['B']</t>
-  </si>
-  <si>
-    <t>iluminaçãoZoada1.jpeg</t>
-  </si>
-  <si>
-    <t>Total: 0</t>
-  </si>
-  <si>
-    <t>Total: 12</t>
-  </si>
-  <si>
-    <t>2-['-']</t>
-  </si>
-  <si>
-    <t>3-['-']</t>
-  </si>
-  <si>
-    <t>4-['-']</t>
-  </si>
-  <si>
-    <t>5-['-']</t>
-  </si>
-  <si>
-    <t>6-['-']</t>
-  </si>
-  <si>
-    <t>8-['D']</t>
-  </si>
-  <si>
-    <t>9-['C']</t>
-  </si>
-  <si>
-    <t>10-['E']</t>
-  </si>
-  <si>
-    <t>11-['A']</t>
-  </si>
-  <si>
-    <t>meioZoado.png</t>
-  </si>
-  <si>
-    <t>gabaritoComErro.jpeg</t>
-  </si>
-  <si>
-    <t>1-['D', 'E']</t>
-  </si>
-  <si>
-    <t>20-['A', 'D', 'E']</t>
-  </si>
-  <si>
-    <t>3.jpeg</t>
-  </si>
-  <si>
-    <t>clahe_2.jpeg</t>
-  </si>
-  <si>
-    <t>23-['D', 'B']</t>
-  </si>
-  <si>
-    <t>25-['B']</t>
-  </si>
-  <si>
-    <t>41-['C']</t>
-  </si>
-  <si>
-    <t>45-['B']</t>
-  </si>
-  <si>
-    <t>46-['D', 'D']</t>
-  </si>
-  <si>
-    <t>47-['A']</t>
-  </si>
-  <si>
-    <t>48-['E', 'E']</t>
-  </si>
-  <si>
-    <t>testeComErro5.jpeg</t>
-  </si>
-  <si>
-    <t>Total: 43</t>
-  </si>
-  <si>
-    <t>Total: 7</t>
-  </si>
-  <si>
     <t>31-['-']</t>
   </si>
   <si>
     <t>gabaritoNovo.jpeg</t>
   </si>
   <si>
-    <t>Total: 50</t>
-  </si>
-  <si>
     <t>comErro1.jpeg</t>
   </si>
   <si>
-    <t>Total: 36</t>
-  </si>
-  <si>
-    <t>Total: 8</t>
-  </si>
-  <si>
-    <t>42-['B']</t>
-  </si>
-  <si>
-    <t>43-['E']</t>
+    <t>Total: 37</t>
   </si>
   <si>
     <t>1.jpeg</t>
@@ -1458,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
         <v>61</v>
@@ -1515,81 +1476,84 @@
         <v>7</v>
       </c>
       <c r="V14" t="s">
+        <v>76</v>
+      </c>
+      <c r="W14" t="s">
         <v>77</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>78</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>79</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Z14" t="s">
         <v>8</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AA14" t="s">
         <v>80</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AB14" t="s">
         <v>81</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>82</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>83</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>84</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AF14" t="s">
         <v>85</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AG14" t="s">
         <v>86</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="AH14" t="s">
         <v>87</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AI14" t="s">
         <v>88</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AJ14" t="s">
         <v>89</v>
       </c>
-      <c r="AJ14" t="s">
+      <c r="AK14" t="s">
         <v>90</v>
       </c>
-      <c r="AK14" t="s">
+      <c r="AL14" t="s">
         <v>91</v>
       </c>
-      <c r="AL14" t="s">
+      <c r="AM14" t="s">
         <v>92</v>
       </c>
-      <c r="AM14" t="s">
+      <c r="AN14" t="s">
         <v>9</v>
       </c>
-      <c r="AN14" t="s">
+      <c r="AO14" t="s">
         <v>93</v>
       </c>
-      <c r="AO14" t="s">
+      <c r="AP14" t="s">
         <v>94</v>
       </c>
-      <c r="AP14" t="s">
+      <c r="AQ14" t="s">
         <v>95</v>
       </c>
-      <c r="AQ14" t="s">
+      <c r="AR14" t="s">
         <v>96</v>
       </c>
-      <c r="AR14" t="s">
+      <c r="AS14" t="s">
         <v>97</v>
       </c>
-      <c r="AS14" t="s">
+      <c r="AT14" t="s">
         <v>10</v>
       </c>
-      <c r="AT14" t="s">
+      <c r="AU14" t="s">
         <v>98</v>
       </c>
-      <c r="AU14" t="s">
+      <c r="AV14" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1598,7 +1562,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
         <v>100</v>
@@ -1613,26 +1577,23 @@
         <v>103</v>
       </c>
       <c r="H15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:52">
+    <row r="17" spans="1:53">
       <c r="A17" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:52">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53">
       <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E18" t="s">
         <v>61</v>
@@ -1692,115 +1653,115 @@
         <v>75</v>
       </c>
       <c r="X18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Y18" t="s">
         <v>7</v>
       </c>
       <c r="Z18" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA18" t="s">
         <v>77</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AB18" t="s">
         <v>78</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AC18" t="s">
         <v>79</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AD18" t="s">
         <v>8</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AE18" t="s">
         <v>80</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AF18" t="s">
         <v>81</v>
       </c>
-      <c r="AF18" t="s">
+      <c r="AG18" t="s">
         <v>82</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AH18" t="s">
         <v>83</v>
       </c>
-      <c r="AH18" t="s">
+      <c r="AI18" t="s">
         <v>84</v>
       </c>
-      <c r="AI18" t="s">
+      <c r="AJ18" t="s">
         <v>85</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AK18" t="s">
         <v>86</v>
       </c>
-      <c r="AK18" t="s">
+      <c r="AL18" t="s">
         <v>87</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AM18" t="s">
         <v>88</v>
       </c>
-      <c r="AM18" t="s">
+      <c r="AN18" t="s">
         <v>89</v>
       </c>
-      <c r="AN18" t="s">
+      <c r="AO18" t="s">
         <v>90</v>
       </c>
-      <c r="AO18" t="s">
+      <c r="AP18" t="s">
         <v>91</v>
       </c>
-      <c r="AP18" t="s">
+      <c r="AQ18" t="s">
         <v>92</v>
       </c>
-      <c r="AQ18" t="s">
+      <c r="AR18" t="s">
         <v>9</v>
       </c>
-      <c r="AR18" t="s">
+      <c r="AS18" t="s">
         <v>93</v>
       </c>
-      <c r="AS18" t="s">
+      <c r="AT18" t="s">
         <v>94</v>
       </c>
-      <c r="AT18" t="s">
+      <c r="AU18" t="s">
         <v>95</v>
       </c>
-      <c r="AU18" t="s">
+      <c r="AV18" t="s">
         <v>96</v>
       </c>
-      <c r="AV18" t="s">
+      <c r="AW18" t="s">
         <v>97</v>
       </c>
-      <c r="AW18" t="s">
+      <c r="AX18" t="s">
         <v>10</v>
       </c>
-      <c r="AX18" t="s">
+      <c r="AY18" t="s">
         <v>98</v>
       </c>
-      <c r="AY18" t="s">
+      <c r="AZ18" t="s">
         <v>11</v>
       </c>
-      <c r="AZ18" t="s">
+      <c r="BA18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:52">
+    <row r="19" spans="1:53">
       <c r="B19" t="s">
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:52">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:53">
       <c r="A21" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:52">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:53">
       <c r="B22" t="s">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
         <v>61</v>
@@ -1857,90 +1818,93 @@
         <v>7</v>
       </c>
       <c r="V22" t="s">
+        <v>76</v>
+      </c>
+      <c r="W22" t="s">
         <v>77</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
         <v>78</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>79</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>8</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AA22" t="s">
         <v>80</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AB22" t="s">
         <v>81</v>
       </c>
-      <c r="AB22" t="s">
+      <c r="AC22" t="s">
         <v>82</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AD22" t="s">
         <v>83</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>84</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AF22" t="s">
         <v>85</v>
       </c>
-      <c r="AF22" t="s">
+      <c r="AG22" t="s">
         <v>86</v>
       </c>
-      <c r="AG22" t="s">
+      <c r="AH22" t="s">
         <v>87</v>
       </c>
-      <c r="AH22" t="s">
+      <c r="AI22" t="s">
         <v>88</v>
       </c>
-      <c r="AI22" t="s">
+      <c r="AJ22" t="s">
         <v>89</v>
       </c>
-      <c r="AJ22" t="s">
+      <c r="AK22" t="s">
         <v>90</v>
       </c>
-      <c r="AK22" t="s">
+      <c r="AL22" t="s">
         <v>91</v>
       </c>
-      <c r="AL22" t="s">
+      <c r="AM22" t="s">
         <v>92</v>
       </c>
-      <c r="AM22" t="s">
+      <c r="AN22" t="s">
         <v>9</v>
       </c>
-      <c r="AN22" t="s">
+      <c r="AO22" t="s">
         <v>93</v>
       </c>
-      <c r="AO22" t="s">
+      <c r="AP22" t="s">
         <v>94</v>
       </c>
-      <c r="AP22" t="s">
+      <c r="AQ22" t="s">
         <v>95</v>
       </c>
-      <c r="AQ22" t="s">
+      <c r="AR22" t="s">
         <v>96</v>
       </c>
-      <c r="AR22" t="s">
+      <c r="AS22" t="s">
         <v>97</v>
       </c>
-      <c r="AS22" t="s">
+      <c r="AT22" t="s">
         <v>10</v>
       </c>
-      <c r="AT22" t="s">
+      <c r="AU22" t="s">
         <v>98</v>
       </c>
-      <c r="AU22" t="s">
+      <c r="AV22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:52">
+    <row r="23" spans="1:53">
       <c r="B23" t="s">
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D23" t="s">
         <v>100</v>
@@ -1955,18 +1919,15 @@
         <v>103</v>
       </c>
       <c r="H23" t="s">
-        <v>108</v>
-      </c>
-      <c r="I23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:52">
+    <row r="25" spans="1:53">
       <c r="A25" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:52">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:53">
       <c r="B26" t="s">
         <v>1</v>
       </c>
@@ -2004,7 +1965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:52">
+    <row r="27" spans="1:53">
       <c r="B27" t="s">
         <v>13</v>
       </c>
@@ -2132,12 +2093,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:52">
+    <row r="29" spans="1:53">
       <c r="A29" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:52">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:53">
       <c r="B30" t="s">
         <v>1</v>
       </c>
@@ -2172,7 +2133,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:52">
+    <row r="31" spans="1:53">
       <c r="B31" t="s">
         <v>13</v>
       </c>
@@ -2180,109 +2141,109 @@
         <v>57</v>
       </c>
       <c r="D31" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" t="s">
+        <v>116</v>
+      </c>
+      <c r="G31" t="s">
         <v>117</v>
       </c>
-      <c r="E31" t="s">
+      <c r="H31" t="s">
         <v>118</v>
       </c>
-      <c r="F31" t="s">
+      <c r="I31" t="s">
         <v>119</v>
       </c>
-      <c r="G31" t="s">
+      <c r="J31" t="s">
         <v>120</v>
-      </c>
-      <c r="H31" t="s">
-        <v>121</v>
-      </c>
-      <c r="I31" t="s">
-        <v>122</v>
-      </c>
-      <c r="J31" t="s">
-        <v>123</v>
       </c>
       <c r="K31" t="s">
         <v>21</v>
       </c>
       <c r="L31" t="s">
+        <v>121</v>
+      </c>
+      <c r="M31" t="s">
+        <v>122</v>
+      </c>
+      <c r="N31" t="s">
+        <v>123</v>
+      </c>
+      <c r="O31" t="s">
         <v>124</v>
       </c>
-      <c r="M31" t="s">
+      <c r="P31" t="s">
         <v>125</v>
       </c>
-      <c r="N31" t="s">
+      <c r="Q31" t="s">
         <v>126</v>
       </c>
-      <c r="O31" t="s">
+      <c r="R31" t="s">
         <v>127</v>
       </c>
-      <c r="P31" t="s">
+      <c r="S31" t="s">
         <v>128</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="T31" t="s">
         <v>129</v>
-      </c>
-      <c r="R31" t="s">
-        <v>130</v>
-      </c>
-      <c r="S31" t="s">
-        <v>131</v>
-      </c>
-      <c r="T31" t="s">
-        <v>132</v>
       </c>
       <c r="U31" t="s">
         <v>103</v>
       </c>
       <c r="V31" t="s">
+        <v>130</v>
+      </c>
+      <c r="W31" t="s">
+        <v>131</v>
+      </c>
+      <c r="X31" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y31" t="s">
         <v>133</v>
       </c>
-      <c r="W31" t="s">
+      <c r="Z31" t="s">
         <v>134</v>
       </c>
-      <c r="X31" t="s">
+      <c r="AA31" t="s">
         <v>135</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="AB31" t="s">
         <v>136</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>138</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>139</v>
       </c>
       <c r="AC31" t="s">
         <v>37</v>
       </c>
       <c r="AD31" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AE31" t="s">
         <v>40</v>
       </c>
       <c r="AF31" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>139</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI31" t="s">
         <v>141</v>
       </c>
-      <c r="AG31" t="s">
+      <c r="AJ31" t="s">
         <v>142</v>
       </c>
-      <c r="AH31" t="s">
+      <c r="AK31" t="s">
         <v>143</v>
       </c>
-      <c r="AI31" t="s">
+      <c r="AL31" t="s">
         <v>144</v>
-      </c>
-      <c r="AJ31" t="s">
-        <v>145</v>
-      </c>
-      <c r="AK31" t="s">
-        <v>146</v>
-      </c>
-      <c r="AL31" t="s">
-        <v>147</v>
       </c>
       <c r="AM31" t="s">
         <v>48</v>
@@ -2291,81 +2252,63 @@
         <v>58</v>
       </c>
       <c r="AO31" t="s">
+        <v>145</v>
+      </c>
+      <c r="AP31" t="s">
+        <v>146</v>
+      </c>
+      <c r="AQ31" t="s">
+        <v>147</v>
+      </c>
+      <c r="AR31" t="s">
         <v>148</v>
       </c>
-      <c r="AP31" t="s">
+    </row>
+    <row r="33" spans="1:53">
+      <c r="A33" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="AQ31" t="s">
-        <v>150</v>
-      </c>
-      <c r="AR31" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:52">
-      <c r="A33" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:52">
+    </row>
+    <row r="34" spans="1:53">
       <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="35" spans="1:52">
+        <v>150</v>
+      </c>
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:53">
       <c r="B35" t="s">
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D35" t="s">
         <v>100</v>
       </c>
       <c r="E35" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:53">
+      <c r="A37" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F35" t="s">
-        <v>156</v>
-      </c>
-      <c r="G35" t="s">
-        <v>157</v>
-      </c>
-      <c r="H35" t="s">
-        <v>158</v>
-      </c>
-      <c r="I35" t="s">
-        <v>159</v>
-      </c>
-      <c r="J35" t="s">
-        <v>20</v>
-      </c>
-      <c r="K35" t="s">
-        <v>160</v>
-      </c>
-      <c r="L35" t="s">
-        <v>161</v>
-      </c>
-      <c r="M35" t="s">
-        <v>162</v>
-      </c>
-      <c r="N35" t="s">
-        <v>163</v>
-      </c>
-      <c r="O35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:52">
-      <c r="A37" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38" spans="1:52">
+    </row>
+    <row r="38" spans="1:53">
       <c r="B38" t="s">
         <v>1</v>
       </c>
@@ -2403,7 +2346,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:52">
+    <row r="39" spans="1:53">
       <c r="B39" t="s">
         <v>13</v>
       </c>
@@ -2531,12 +2474,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:52">
+    <row r="41" spans="1:53">
       <c r="A41" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="1:52">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:53">
       <c r="B42" t="s">
         <v>1</v>
       </c>
@@ -2574,7 +2517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:52">
+    <row r="43" spans="1:53">
       <c r="B43" t="s">
         <v>13</v>
       </c>
@@ -2582,7 +2525,7 @@
         <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E43" t="s">
         <v>16</v>
@@ -2627,7 +2570,7 @@
         <v>29</v>
       </c>
       <c r="S43" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="T43" t="s">
         <v>31</v>
@@ -2702,20 +2645,20 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:52">
+    <row r="45" spans="1:53">
       <c r="A45" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="46" spans="1:52">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:53">
       <c r="B46" t="s">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D46" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E46" t="s">
         <v>61</v>
@@ -2775,107 +2718,107 @@
         <v>75</v>
       </c>
       <c r="X46" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Y46" t="s">
         <v>7</v>
       </c>
       <c r="Z46" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA46" t="s">
         <v>77</v>
       </c>
-      <c r="AA46" t="s">
+      <c r="AB46" t="s">
         <v>78</v>
       </c>
-      <c r="AB46" t="s">
+      <c r="AC46" t="s">
         <v>79</v>
       </c>
-      <c r="AC46" t="s">
+      <c r="AD46" t="s">
         <v>8</v>
       </c>
-      <c r="AD46" t="s">
+      <c r="AE46" t="s">
         <v>80</v>
       </c>
-      <c r="AE46" t="s">
+      <c r="AF46" t="s">
         <v>81</v>
       </c>
-      <c r="AF46" t="s">
+      <c r="AG46" t="s">
         <v>82</v>
       </c>
-      <c r="AG46" t="s">
+      <c r="AH46" t="s">
         <v>83</v>
       </c>
-      <c r="AH46" t="s">
+      <c r="AI46" t="s">
         <v>84</v>
       </c>
-      <c r="AI46" t="s">
+      <c r="AJ46" t="s">
         <v>85</v>
       </c>
-      <c r="AJ46" t="s">
+      <c r="AK46" t="s">
         <v>86</v>
       </c>
-      <c r="AK46" t="s">
+      <c r="AL46" t="s">
         <v>87</v>
       </c>
-      <c r="AL46" t="s">
+      <c r="AM46" t="s">
         <v>88</v>
       </c>
-      <c r="AM46" t="s">
+      <c r="AN46" t="s">
         <v>89</v>
       </c>
-      <c r="AN46" t="s">
+      <c r="AO46" t="s">
         <v>90</v>
       </c>
-      <c r="AO46" t="s">
+      <c r="AP46" t="s">
         <v>91</v>
       </c>
-      <c r="AP46" t="s">
+      <c r="AQ46" t="s">
         <v>92</v>
       </c>
-      <c r="AQ46" t="s">
+      <c r="AR46" t="s">
         <v>9</v>
       </c>
-      <c r="AR46" t="s">
+      <c r="AS46" t="s">
         <v>93</v>
       </c>
-      <c r="AS46" t="s">
+      <c r="AT46" t="s">
         <v>94</v>
       </c>
-      <c r="AT46" t="s">
+      <c r="AU46" t="s">
         <v>95</v>
       </c>
-      <c r="AU46" t="s">
+      <c r="AV46" t="s">
         <v>96</v>
       </c>
-      <c r="AV46" t="s">
+      <c r="AW46" t="s">
         <v>97</v>
       </c>
-      <c r="AW46" t="s">
+      <c r="AX46" t="s">
         <v>10</v>
       </c>
-      <c r="AX46" t="s">
+      <c r="AY46" t="s">
         <v>98</v>
       </c>
-      <c r="AY46" t="s">
+      <c r="AZ46" t="s">
         <v>11</v>
       </c>
-      <c r="AZ46" t="s">
+      <c r="BA46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:52">
+    <row r="47" spans="1:53">
       <c r="B47" t="s">
         <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:53">
       <c r="A49" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:53">
@@ -2883,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
       <c r="D50" t="s">
         <v>67</v>
@@ -2901,6 +2844,9 @@
         <v>94</v>
       </c>
       <c r="I50" t="s">
+        <v>97</v>
+      </c>
+      <c r="J50" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2909,118 +2855,118 @@
         <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>162</v>
       </c>
       <c r="D51" t="s">
+        <v>114</v>
+      </c>
+      <c r="E51" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" t="s">
+        <v>116</v>
+      </c>
+      <c r="G51" t="s">
         <v>117</v>
       </c>
-      <c r="E51" t="s">
+      <c r="H51" t="s">
         <v>118</v>
       </c>
-      <c r="F51" t="s">
+      <c r="I51" t="s">
         <v>119</v>
       </c>
-      <c r="G51" t="s">
+      <c r="J51" t="s">
         <v>120</v>
-      </c>
-      <c r="H51" t="s">
-        <v>121</v>
-      </c>
-      <c r="I51" t="s">
-        <v>122</v>
-      </c>
-      <c r="J51" t="s">
-        <v>123</v>
       </c>
       <c r="K51" t="s">
         <v>21</v>
       </c>
       <c r="L51" t="s">
+        <v>121</v>
+      </c>
+      <c r="M51" t="s">
+        <v>122</v>
+      </c>
+      <c r="N51" t="s">
+        <v>123</v>
+      </c>
+      <c r="O51" t="s">
         <v>124</v>
       </c>
-      <c r="M51" t="s">
+      <c r="P51" t="s">
         <v>125</v>
       </c>
-      <c r="N51" t="s">
+      <c r="Q51" t="s">
         <v>126</v>
       </c>
-      <c r="O51" t="s">
+      <c r="R51" t="s">
         <v>127</v>
       </c>
-      <c r="P51" t="s">
+      <c r="S51" t="s">
         <v>128</v>
       </c>
-      <c r="Q51" t="s">
+      <c r="T51" t="s">
         <v>129</v>
-      </c>
-      <c r="R51" t="s">
-        <v>130</v>
-      </c>
-      <c r="S51" t="s">
-        <v>131</v>
-      </c>
-      <c r="T51" t="s">
-        <v>132</v>
       </c>
       <c r="U51" t="s">
         <v>103</v>
       </c>
       <c r="V51" t="s">
+        <v>130</v>
+      </c>
+      <c r="W51" t="s">
+        <v>163</v>
+      </c>
+      <c r="X51" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y51" t="s">
         <v>133</v>
       </c>
-      <c r="W51" t="s">
-        <v>170</v>
-      </c>
-      <c r="X51" t="s">
+      <c r="Z51" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA51" t="s">
         <v>135</v>
       </c>
-      <c r="Y51" t="s">
-        <v>171</v>
-      </c>
-      <c r="Z51" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA51" t="s">
-        <v>138</v>
-      </c>
       <c r="AB51" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AC51" t="s">
         <v>37</v>
       </c>
       <c r="AD51" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AE51" t="s">
         <v>40</v>
       </c>
       <c r="AF51" t="s">
+        <v>138</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>139</v>
+      </c>
+      <c r="AH51" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI51" t="s">
         <v>141</v>
       </c>
-      <c r="AG51" t="s">
+      <c r="AJ51" t="s">
         <v>142</v>
       </c>
-      <c r="AH51" t="s">
+      <c r="AK51" t="s">
         <v>143</v>
       </c>
-      <c r="AI51" t="s">
+      <c r="AL51" t="s">
         <v>144</v>
-      </c>
-      <c r="AJ51" t="s">
-        <v>145</v>
-      </c>
-      <c r="AK51" t="s">
-        <v>146</v>
-      </c>
-      <c r="AL51" t="s">
-        <v>147</v>
       </c>
       <c r="AM51" t="s">
         <v>48</v>
       </c>
       <c r="AN51" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="AO51" t="s">
         <v>49</v>
@@ -3029,24 +2975,21 @@
         <v>51</v>
       </c>
       <c r="AQ51" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="AR51" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="AS51" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="AT51" t="s">
-        <v>176</v>
-      </c>
-      <c r="AU51" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:53">
       <c r="A53" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:53">
@@ -3054,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D54" t="s">
         <v>61</v>
@@ -3111,78 +3054,81 @@
         <v>7</v>
       </c>
       <c r="V54" t="s">
+        <v>76</v>
+      </c>
+      <c r="W54" t="s">
         <v>77</v>
       </c>
-      <c r="W54" t="s">
+      <c r="X54" t="s">
         <v>78</v>
       </c>
-      <c r="X54" t="s">
+      <c r="Y54" t="s">
         <v>79</v>
       </c>
-      <c r="Y54" t="s">
+      <c r="Z54" t="s">
         <v>8</v>
       </c>
-      <c r="Z54" t="s">
+      <c r="AA54" t="s">
         <v>80</v>
       </c>
-      <c r="AA54" t="s">
+      <c r="AB54" t="s">
         <v>81</v>
       </c>
-      <c r="AB54" t="s">
+      <c r="AC54" t="s">
         <v>82</v>
       </c>
-      <c r="AC54" t="s">
+      <c r="AD54" t="s">
         <v>84</v>
       </c>
-      <c r="AD54" t="s">
+      <c r="AE54" t="s">
         <v>85</v>
       </c>
-      <c r="AE54" t="s">
+      <c r="AF54" t="s">
         <v>86</v>
       </c>
-      <c r="AF54" t="s">
+      <c r="AG54" t="s">
         <v>87</v>
       </c>
-      <c r="AG54" t="s">
+      <c r="AH54" t="s">
         <v>88</v>
       </c>
-      <c r="AH54" t="s">
+      <c r="AI54" t="s">
         <v>89</v>
       </c>
-      <c r="AI54" t="s">
+      <c r="AJ54" t="s">
         <v>90</v>
       </c>
-      <c r="AJ54" t="s">
+      <c r="AK54" t="s">
         <v>91</v>
       </c>
-      <c r="AK54" t="s">
+      <c r="AL54" t="s">
         <v>92</v>
       </c>
-      <c r="AL54" t="s">
+      <c r="AM54" t="s">
         <v>9</v>
       </c>
-      <c r="AM54" t="s">
+      <c r="AN54" t="s">
         <v>93</v>
       </c>
-      <c r="AN54" t="s">
+      <c r="AO54" t="s">
         <v>94</v>
       </c>
-      <c r="AO54" t="s">
+      <c r="AP54" t="s">
         <v>95</v>
       </c>
-      <c r="AP54" t="s">
+      <c r="AQ54" t="s">
         <v>96</v>
       </c>
-      <c r="AQ54" t="s">
+      <c r="AR54" t="s">
         <v>97</v>
       </c>
-      <c r="AR54" t="s">
+      <c r="AS54" t="s">
         <v>10</v>
       </c>
-      <c r="AS54" t="s">
+      <c r="AT54" t="s">
         <v>98</v>
       </c>
-      <c r="AT54" t="s">
+      <c r="AU54" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3191,7 +3137,7 @@
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D55" t="s">
         <v>100</v>
@@ -3206,18 +3152,15 @@
         <v>103</v>
       </c>
       <c r="H55" t="s">
-        <v>108</v>
+        <v>171</v>
       </c>
       <c r="I55" t="s">
-        <v>180</v>
-      </c>
-      <c r="J55" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:53">
       <c r="A57" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:53">
@@ -3225,10 +3168,10 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="D58" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E58" t="s">
         <v>61</v>
@@ -3288,7 +3231,7 @@
         <v>75</v>
       </c>
       <c r="X58" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Y58" t="s">
         <v>7</v>
@@ -3383,12 +3326,12 @@
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:53">
       <c r="A61" s="1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:53">
@@ -3396,7 +3339,7 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D62" t="s">
         <v>61</v>
@@ -3505,6 +3448,9 @@
       </c>
       <c r="AM62" t="s">
         <v>92</v>
+      </c>
+      <c r="AN62" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:53">
@@ -3512,7 +3458,7 @@
         <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="D63" t="s">
         <v>100</v>
@@ -3526,22 +3472,10 @@
       <c r="G63" t="s">
         <v>103</v>
       </c>
-      <c r="H63" t="s">
-        <v>58</v>
-      </c>
-      <c r="I63" t="s">
-        <v>186</v>
-      </c>
-      <c r="J63" t="s">
-        <v>187</v>
-      </c>
-      <c r="K63" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="65" spans="1:53">
       <c r="A65" s="1" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66" spans="1:53">
@@ -3549,10 +3483,10 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="D66" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E66" t="s">
         <v>61</v>
@@ -3612,7 +3546,7 @@
         <v>75</v>
       </c>
       <c r="X66" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Y66" t="s">
         <v>7</v>
@@ -3707,12 +3641,12 @@
         <v>13</v>
       </c>
       <c r="C67" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
     </row>
     <row r="69" spans="1:53">
       <c r="A69" s="1" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="70" spans="1:53">
@@ -3720,10 +3654,10 @@
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D70" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E70" t="s">
         <v>61</v>
@@ -3783,90 +3717,93 @@
         <v>75</v>
       </c>
       <c r="X70" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Y70" t="s">
         <v>7</v>
       </c>
       <c r="Z70" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA70" t="s">
         <v>77</v>
       </c>
-      <c r="AA70" t="s">
+      <c r="AB70" t="s">
         <v>78</v>
       </c>
-      <c r="AB70" t="s">
+      <c r="AC70" t="s">
         <v>79</v>
       </c>
-      <c r="AC70" t="s">
+      <c r="AD70" t="s">
         <v>8</v>
       </c>
-      <c r="AD70" t="s">
+      <c r="AE70" t="s">
         <v>80</v>
       </c>
-      <c r="AE70" t="s">
+      <c r="AF70" t="s">
         <v>81</v>
       </c>
-      <c r="AF70" t="s">
+      <c r="AG70" t="s">
         <v>82</v>
       </c>
-      <c r="AG70" t="s">
+      <c r="AH70" t="s">
         <v>83</v>
       </c>
-      <c r="AH70" t="s">
+      <c r="AI70" t="s">
         <v>84</v>
       </c>
-      <c r="AI70" t="s">
+      <c r="AJ70" t="s">
         <v>85</v>
       </c>
-      <c r="AJ70" t="s">
+      <c r="AK70" t="s">
         <v>86</v>
       </c>
-      <c r="AK70" t="s">
+      <c r="AL70" t="s">
         <v>87</v>
       </c>
-      <c r="AL70" t="s">
+      <c r="AM70" t="s">
         <v>88</v>
       </c>
-      <c r="AM70" t="s">
+      <c r="AN70" t="s">
         <v>89</v>
       </c>
-      <c r="AN70" t="s">
+      <c r="AO70" t="s">
         <v>90</v>
       </c>
-      <c r="AO70" t="s">
+      <c r="AP70" t="s">
         <v>91</v>
       </c>
-      <c r="AP70" t="s">
+      <c r="AQ70" t="s">
         <v>92</v>
       </c>
-      <c r="AQ70" t="s">
+      <c r="AR70" t="s">
         <v>9</v>
       </c>
-      <c r="AR70" t="s">
+      <c r="AS70" t="s">
         <v>93</v>
       </c>
-      <c r="AS70" t="s">
+      <c r="AT70" t="s">
         <v>94</v>
       </c>
-      <c r="AT70" t="s">
+      <c r="AU70" t="s">
         <v>95</v>
       </c>
-      <c r="AU70" t="s">
+      <c r="AV70" t="s">
         <v>96</v>
       </c>
-      <c r="AV70" t="s">
+      <c r="AW70" t="s">
         <v>97</v>
       </c>
-      <c r="AW70" t="s">
+      <c r="AX70" t="s">
         <v>10</v>
       </c>
-      <c r="AX70" t="s">
+      <c r="AY70" t="s">
         <v>98</v>
       </c>
-      <c r="AY70" t="s">
+      <c r="AZ70" t="s">
         <v>11</v>
       </c>
-      <c r="AZ70" t="s">
+      <c r="BA70" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3875,15 +3812,12 @@
         <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>113</v>
-      </c>
-      <c r="D71" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:53">
       <c r="A73" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:53">
@@ -4054,7 +3988,7 @@
     </row>
     <row r="77" spans="1:53">
       <c r="A77" s="1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="78" spans="1:53">
@@ -4062,7 +3996,7 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="D78" t="s">
         <v>61</v>
@@ -4119,81 +4053,84 @@
         <v>7</v>
       </c>
       <c r="V78" t="s">
+        <v>76</v>
+      </c>
+      <c r="W78" t="s">
         <v>77</v>
       </c>
-      <c r="W78" t="s">
+      <c r="X78" t="s">
         <v>78</v>
       </c>
-      <c r="X78" t="s">
+      <c r="Y78" t="s">
         <v>79</v>
       </c>
-      <c r="Y78" t="s">
+      <c r="Z78" t="s">
         <v>8</v>
       </c>
-      <c r="Z78" t="s">
+      <c r="AA78" t="s">
         <v>80</v>
       </c>
-      <c r="AA78" t="s">
+      <c r="AB78" t="s">
         <v>81</v>
       </c>
-      <c r="AB78" t="s">
+      <c r="AC78" t="s">
         <v>82</v>
       </c>
-      <c r="AC78" t="s">
+      <c r="AD78" t="s">
         <v>83</v>
       </c>
-      <c r="AD78" t="s">
+      <c r="AE78" t="s">
         <v>84</v>
       </c>
-      <c r="AE78" t="s">
+      <c r="AF78" t="s">
         <v>85</v>
       </c>
-      <c r="AF78" t="s">
+      <c r="AG78" t="s">
         <v>86</v>
       </c>
-      <c r="AG78" t="s">
+      <c r="AH78" t="s">
         <v>87</v>
       </c>
-      <c r="AH78" t="s">
+      <c r="AI78" t="s">
         <v>88</v>
       </c>
-      <c r="AI78" t="s">
+      <c r="AJ78" t="s">
         <v>89</v>
       </c>
-      <c r="AJ78" t="s">
+      <c r="AK78" t="s">
         <v>90</v>
       </c>
-      <c r="AK78" t="s">
+      <c r="AL78" t="s">
         <v>91</v>
       </c>
-      <c r="AL78" t="s">
+      <c r="AM78" t="s">
         <v>92</v>
       </c>
-      <c r="AM78" t="s">
+      <c r="AN78" t="s">
         <v>9</v>
       </c>
-      <c r="AN78" t="s">
+      <c r="AO78" t="s">
         <v>93</v>
       </c>
-      <c r="AO78" t="s">
+      <c r="AP78" t="s">
         <v>94</v>
       </c>
-      <c r="AP78" t="s">
+      <c r="AQ78" t="s">
         <v>95</v>
       </c>
-      <c r="AQ78" t="s">
+      <c r="AR78" t="s">
         <v>96</v>
       </c>
-      <c r="AR78" t="s">
+      <c r="AS78" t="s">
         <v>97</v>
       </c>
-      <c r="AS78" t="s">
+      <c r="AT78" t="s">
         <v>10</v>
       </c>
-      <c r="AT78" t="s">
+      <c r="AU78" t="s">
         <v>98</v>
       </c>
-      <c r="AU78" t="s">
+      <c r="AV78" t="s">
         <v>11</v>
       </c>
     </row>
@@ -4202,7 +4139,7 @@
         <v>13</v>
       </c>
       <c r="C79" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D79" t="s">
         <v>100</v>
@@ -4217,9 +4154,6 @@
         <v>103</v>
       </c>
       <c r="H79" t="s">
-        <v>108</v>
-      </c>
-      <c r="I79" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>